<commit_message>
add and update all files
</commit_message>
<xml_diff>
--- a/label_count.xlsx
+++ b/label_count.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>42902</v>
+        <v>26880</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>12965</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="4">
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>891</v>
+        <v>21741</v>
       </c>
     </row>
     <row r="5">
@@ -469,15 +469,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4700</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>629</v>
+        <v>11008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>